<commit_message>
- Authenticate Sequence & State
</commit_message>
<xml_diff>
--- a/Timesheet and MOM/ตารางบันทึกการมีส่วนร่วมของสมาชิกในกลุ่ม6.xlsx
+++ b/Timesheet and MOM/ตารางบันทึกการมีส่วนร่วมของสมาชิกในกลุ่ม6.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\BubbleBeeDoc\Timesheet and MOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="810" windowWidth="19575" windowHeight="7080" activeTab="7"/>
+    <workbookView xWindow="390" yWindow="810" windowWidth="19575" windowHeight="7080" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Week#1" sheetId="2" r:id="rId1"/>
@@ -15,11 +20,12 @@
     <sheet name="Week#5" sheetId="8" r:id="rId6"/>
     <sheet name="Week#7" sheetId="10" r:id="rId7"/>
     <sheet name="Week#8" sheetId="11" r:id="rId8"/>
-    <sheet name="Instruction" sheetId="1" r:id="rId9"/>
-    <sheet name="TeamMember" sheetId="7" r:id="rId10"/>
+    <sheet name="Week#9" sheetId="12" r:id="rId9"/>
+    <sheet name="Instruction" sheetId="1" r:id="rId10"/>
+    <sheet name="TeamMember" sheetId="7" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week#1'!$A$1:$H$17</definedName>
@@ -28,12 +34,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Week#3'!$A$1:$H$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Week#4'!$A$1:$H$17</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="173">
   <si>
     <t>วิธีการกรอก</t>
   </si>
@@ -616,6 +622,20 @@
   </si>
   <si>
     <t xml:space="preserve">- ความเข้าใจในการทำ CRC และ Class Diagram ยังไม่ตรงกันจึงต้องมีการทวนสอบกันเป็นระยะ </t>
+  </si>
+  <si>
+    <t>System Software Design V0.4</t>
+  </si>
+  <si>
+    <t>- ประชุมปรึกษาปัญหาที่เกิดจากการทำงานรอบที่แล้ว มอบหมายงาน และอธิบายเนื้องานที่ได้รับมอบหมายกันอาทิตย์นี้
+- จัดทำ Sequence Diagram ระบบตรวจสอบสิทธิ์เข้าใช้งาน (เพิ่มข้อมูลพนักงานใหม่ และตรวจสอบสิทธิ์เข้าใช้งาน)
+- จัดทำ Behavioral State Machine ระบบตรวจสอบสิทธิ์เข้าใช้งาน 
+- รวบรวมเอกสารออกแบบระบบจากสมาชิกภายในกลุ่ม</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+- 
+</t>
   </si>
 </sst>
 </file>
@@ -981,7 +1001,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1016,7 +1036,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1559,6 +1579,42 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3481,7 +3537,7 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -3635,7 +3691,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="130.5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="152.25" x14ac:dyDescent="0.5">
       <c r="A12" s="22">
         <v>3</v>
       </c>
@@ -3766,8 +3822,8 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -3866,7 +3922,7 @@
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
     </row>
-    <row r="10" spans="1:8" ht="87" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="108.75" x14ac:dyDescent="0.5">
       <c r="A10" s="22">
         <v>1</v>
       </c>
@@ -4042,36 +4098,243 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="14.42578125" style="18"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="A2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="A3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="A4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="A5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="A6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="44"/>
+      <c r="F8" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="A10" s="22">
+        <v>1</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22">
+        <f>D10+E10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="G10" s="30"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" ht="153" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="22">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B11" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22">
+        <f t="shared" ref="F11" si="0">D11+E11</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+    </row>
+    <row r="12" spans="1:8" ht="174" x14ac:dyDescent="0.5">
+      <c r="A12" s="22">
+        <v>3</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="22">
+        <v>5</v>
+      </c>
+      <c r="E12" s="22">
+        <v>3</v>
+      </c>
+      <c r="F12" s="22">
+        <f>D12+E12</f>
         <v>8</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="G12" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="A13" s="22">
+        <v>4</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22">
+        <f>D13+E13</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="A14" s="32">
+        <v>5</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22">
+        <f>D14+E14</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="A15" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="22">
+        <f>SUM(F10:F14)</f>
+        <v>8</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1">
+          <x14:formula1>
+            <xm:f>TeamMember!$E$2:$E$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10:B14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>